<commit_message>
api test case updated
</commit_message>
<xml_diff>
--- a/API test cases.xlsx
+++ b/API test cases.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Company Contractor" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28822,7 +28823,7 @@
   <dimension ref="B3:AA1003"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="87" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -56892,4 +56893,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>